<commit_message>
add estimated complexities to ALL instructions
</commit_message>
<xml_diff>
--- a/VarexJSmallScaleEvaluation/complex-inc.IncVarexJ.xlsx
+++ b/VarexJSmallScaleEvaluation/complex-inc.IncVarexJ.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="complex-inc.IncVarexJ" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -1135,11 +1135,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="196675072"/>
-        <c:axId val="145350656"/>
+        <c:axId val="173451264"/>
+        <c:axId val="148471104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="196675072"/>
+        <c:axId val="173451264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1148,7 +1148,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145350656"/>
+        <c:crossAx val="148471104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1156,7 +1156,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145350656"/>
+        <c:axId val="148471104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1167,7 +1167,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196675072"/>
+        <c:crossAx val="173451264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1189,18 +1189,369 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'complex-inc.IncVarexJ'!$D:$D</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1048576"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'complex-inc.IncVarexJ'!$A$1:$A$83</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="83"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="13274624"/>
+        <c:axId val="163928256"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="13274624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="163928256"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="163928256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="13274624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
@@ -1216,6 +1567,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>428626</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1514,7 +1897,7 @@
   <dimension ref="A1:B83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>